<commit_message>
Push fixing link invalid for all API only
</commit_message>
<xml_diff>
--- a/Excel/2.1 Esign - API Only.xlsx
+++ b/Excel/2.1 Esign - API Only.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="12" firstSheet="11" windowHeight="6950" windowWidth="18350"/>
+    <workbookView activeTab="6" firstSheet="6" windowHeight="8130" windowWidth="18350"/>
   </bookViews>
   <sheets>
     <sheet name="API Resend Activation Link" r:id="rId1" sheetId="1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="271">
   <si>
     <t>Status</t>
   </si>
@@ -664,7 +664,7 @@
     <t>http://gdkwebsvr:8080/i/reg?code=kBKMnrRSQajsdIdR8ygeWg%3D%3D</t>
   </si>
   <si>
-    <t>http://gdkwebsvr:8080/i/reg?code=lOMR3L3V85Q18Rspywl4+w%3D%3D</t>
+    <t>http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnnccZenQ%3D%3D</t>
   </si>
   <si>
     <t>Unexecuted</t>
@@ -709,9 +709,6 @@
     <t>;&lt;Tidak bisa mengirimkan OTP ke USERCCRA@GMAIL.COM&gt;</t>
   </si>
   <si>
-    <t>;Key yang diencrypt pada URL tidak terdapat di DB;&lt;Link registrasi tidak valid.&gt;</t>
-  </si>
-  <si>
     <t>Hit dengan email invalid</t>
   </si>
   <si>
@@ -725,8 +722,8 @@
   <si>
     <t>{
     "status": {
-        "code": 7001,
-        "message": "Link registrasi tidak valid."
+        "code": 7019,
+        "message": "Link terpotong pada saat copy dari eSignHub. Mohon copy link dengan benar dan lengkap. Silahkan coba kembali."
     }
 }</t>
   </si>
@@ -743,10 +740,10 @@
     <t>0.14 second</t>
   </si>
   <si>
-    <t>0.375 second</t>
-  </si>
-  <si>
-    <t>1.589 second</t>
+    <t>1.281 second</t>
+  </si>
+  <si>
+    <t>1.191 second</t>
   </si>
   <si>
     <t>OTP before</t>
@@ -755,13 +752,16 @@
     <t>453094</t>
   </si>
   <si>
+    <t>381370</t>
+  </si>
+  <si>
+    <t>OTP latest</t>
+  </si>
+  <si>
     <t>379541</t>
   </si>
   <si>
-    <t>OTP latest</t>
-  </si>
-  <si>
-    <t>305518</t>
+    <t>290839</t>
   </si>
   <si>
     <t>USERCCRA@GMAIL.COM</t>
@@ -770,7 +770,13 @@
     <t>USERBAAA@ESIGNHUB.MY.ID</t>
   </si>
   <si>
-    <t>http://gdkwebsvr:8080/i/reg?code=sP4CMoLA%2FM048p%2BOZCVxrA%3D%3D</t>
+    <t>https://gdkwebsvr:8080/i/reg?code=sP4CMoLA%2FM048p%2BOZCVxrA%3D%3D</t>
+  </si>
+  <si>
+    <t>http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnncZenQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://gdkwebsvr:8080/i/reg?code=Qiw5KLtlFTTA3W5ZBqPoiQ%3D%3D</t>
   </si>
   <si>
     <t>Vendor Code</t>
@@ -786,6 +792,9 @@
   </si>
   <si>
     <t>;&lt;Tidak bisa memverifikasi OTP ke SHIAPA@GMAIL.COM&gt;</t>
+  </si>
+  <si>
+    <t>;Key yang diencrypt pada URL tidak terdapat di DB;&lt;Link registrasi tidak valid.&gt;</t>
   </si>
   <si>
     <t>Hit dengan base url yang salah</t>
@@ -821,6 +830,14 @@
     "status": {
         "code": 7004,
         "message": "Tidak bisa memverifikasi OTP ke SHIAPA@GMAIL.COM"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": {
+        "code": 7001,
+        "message": "Link registrasi tidak valid."
     }
 }</t>
   </si>
@@ -1125,65 +1142,12 @@
     <t>PRIVY</t>
   </si>
   <si>
-    <t>UNexecuted</t>
-  </si>
-  <si>
     <t>{
     "status": {
         "code": 7001,
         "message": "Tidak ada Invitation Link yang cocok dengan data yang disediakan."
     }
 }</t>
-  </si>
-  <si>
-    <t>{
-    "status": {
-        "code": 0,
-        "message": "Success"
-    },
-    "link": "https://gdkwebsvr:8080/i/reg?code=%2FJGfxGISrT%2BXq8U6bMFodw%3D%3D"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": {
-        "code": 0,
-        "message": "Success"
-    },
-    "link": "https://gdkwebsvr:8080/i/reg?code=7UKv4YTYEdm5HJF7gtujKQ%3D%3D"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": {
-        "code": 0,
-        "message": "Success"
-    },
-    "link": "https://gdkwebsvr:8080/i/reg?code=8dF7rtg0rZ8q0D8Ju8EeaQ%3D%3D"
-}</t>
-  </si>
-  <si>
-    <t>0.135 second</t>
-  </si>
-  <si>
-    <t>0.146 second</t>
-  </si>
-  <si>
-    <t>0.136 second</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>{
-    "status": {
-        "code": 0,
-        "message": "Undangan terkirim ke USERCIFH@ESIGNHUB.MY.ID"
-    }
-}</t>
-  </si>
-  <si>
-    <t>USERCIFH@ESIGNHUB.MY.ID</t>
   </si>
   <si>
     <t>{
@@ -1195,9 +1159,6 @@
 }</t>
   </si>
   <si>
-    <t>https://gdkwebsvr:8080/i/reg?code=Yjeyc6uRKvh3nPeVI6j2DQ%3D%3D</t>
-  </si>
-  <si>
     <t>{
     "status": {
         "code": 0,
@@ -1207,12 +1168,6 @@
 }</t>
   </si>
   <si>
-    <t>0.149 second</t>
-  </si>
-  <si>
-    <t>https://gdkwebsvr:8080/i/reg?code=ZaUya1yZ2IODIrwo%2BKJYoQ%3D%3D</t>
-  </si>
-  <si>
     <t>{
     "status": {
         "code": 0,
@@ -1222,7 +1177,42 @@
 }</t>
   </si>
   <si>
-    <t>https://gdkwebsvr:8080/i/reg?code=Qiw5KLtlFTTA3W5ZBqPoiQ%3D%3D</t>
+    <t>0.135 second</t>
+  </si>
+  <si>
+    <t>0.149 second</t>
+  </si>
+  <si>
+    <t>https://gdkwebsvr:8080/i/reg?code=Yjeyc6uRKvh3nPeVI6j2DQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://gdkwebsvr:8080/i/reg?code=ZaUya1yZ2IODIrwo%2BKJYoQ%3D%3D</t>
+  </si>
+  <si>
+    <t>{
+    "status": {
+        "code": 0,
+        "message": "Undangan terkirim ke USERCIFH@ESIGNHUB.MY.ID"
+    }
+}</t>
+  </si>
+  <si>
+    <t>USERCIFH@ESIGNHUB.MY.ID</t>
+  </si>
+  <si>
+    <t>;Link gagal di-decrypt</t>
+  </si>
+  <si>
+    <t>1.154 second</t>
+  </si>
+  <si>
+    <t>;Link gagal di-decrypt;&lt;Link terpotong pada saat copy dari eSignHub. Mohon copy link dengan benar dan lengkap. Silahkan coba kembali.&gt;</t>
+  </si>
+  <si>
+    <t>0.128 second</t>
+  </si>
+  <si>
+    <t>944421</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1262,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1280,7 +1270,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1414,12 +1404,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="134"/>
@@ -1796,10 +1786,10 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="4" fontId="0" numFmtId="0">
@@ -1928,7 +1918,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -1951,6 +1941,8 @@
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="6"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="6"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -2432,10 +2424,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
@@ -2485,19 +2477,19 @@
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2799,22 +2791,22 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="H2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row ht="29" r="3" spans="1:9">
@@ -2825,25 +2817,25 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>118</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2915,22 +2907,22 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E8" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F8" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="G8" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="H8" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="I8" t="s">
         <v>15</v>
@@ -2941,28 +2933,28 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E9" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F9" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G9" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="H9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3025,57 +3017,57 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C13" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D13" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E13" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="F13" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G13" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="H13" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="I13" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="11" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C14" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D14" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E14" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="F14" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="G14" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H14" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="I14" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3093,7 +3085,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>40</v>
@@ -3122,7 +3114,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B17">
         <v>123333</v>
@@ -3381,7 +3373,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -3398,10 +3390,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3470,10 +3462,10 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E9" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3481,10 +3473,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3501,16 +3493,16 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D12" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3532,7 +3524,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="9" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -3720,13 +3712,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="F2" s="14"/>
     </row>
@@ -3735,22 +3727,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3811,19 +3803,19 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D8" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="F8" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G8" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="1" spans="1:7">
@@ -3832,7 +3824,7 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -3841,10 +3833,10 @@
         <v>124</v>
       </c>
       <c r="F9" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G9" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3852,10 +3844,10 @@
         <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="G10" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3988,27 +3980,27 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D18" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E18" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="G18" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="11" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>31</v>
@@ -4042,7 +4034,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>40</v>
@@ -4065,13 +4057,13 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>43</v>
@@ -4120,7 +4112,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>43</v>
@@ -4438,7 +4430,7 @@
   <sheetPr/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G2"/>
     </sheetView>
   </sheetViews>
@@ -4471,7 +4463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row ht="15.25" r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -4490,22 +4482,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4565,19 +4557,19 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="F8" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="G8" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4585,7 +4577,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
         <v>112</v>
@@ -4594,7 +4586,7 @@
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
@@ -4605,13 +4597,13 @@
         <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F10" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G10" t="s">
-        <v>269</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4753,7 +4745,7 @@
         <v>167</v>
       </c>
       <c r="E18" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F18" t="s">
         <v>167</v>
@@ -4764,7 +4756,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="11" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>31</v>
@@ -4798,7 +4790,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>40</v>
@@ -4821,13 +4813,13 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>43</v>
@@ -4876,7 +4868,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>43</v>
@@ -5069,13 +5061,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row ht="29" r="3" spans="1:7">
@@ -5083,22 +5075,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5158,19 +5150,19 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D8" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="F8" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="G8" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row customFormat="1" r="9" spans="1:7">
@@ -5181,13 +5173,13 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E9" t="s">
         <v>124</v>
       </c>
       <c r="F9" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="G9" t="s">
         <v>114</v>
@@ -5323,27 +5315,27 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E17" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="G17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="11" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>31</v>
@@ -5377,7 +5369,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>40</v>
@@ -5400,13 +5392,13 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>43</v>
@@ -5455,7 +5447,7 @@
         <v>43</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>43</v>
@@ -5743,7 +5735,7 @@
     <row r="7" spans="1:1">
       <c r="A7" s="6"/>
     </row>
-    <row customFormat="1" r="8" s="18" spans="1:2">
+    <row customFormat="1" r="8" s="20" spans="1:2">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -5818,22 +5810,22 @@
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5975,20 +5967,20 @@
       <c r="A21" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="21" t="s">
         <v>71</v>
       </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="21" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6042,22 +6034,22 @@
       <c r="A24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="21" t="s">
         <v>77</v>
       </c>
     </row>
@@ -6065,20 +6057,20 @@
       <c r="A25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="21" t="s">
         <v>79</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="21" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6232,7 +6224,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="18" t="s">
         <v>92</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -6266,7 +6258,7 @@
       <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="18" t="s">
         <v>95</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -6289,7 +6281,7 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="18" t="s">
         <v>96</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -6312,25 +6304,25 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="21" t="s">
         <v>99</v>
       </c>
     </row>
@@ -6405,7 +6397,7 @@
       <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="19" t="s">
         <v>100</v>
       </c>
       <c r="B42" s="6"/>
@@ -6655,19 +6647,19 @@
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7154,19 +7146,19 @@
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7224,19 +7216,19 @@
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7348,19 +7340,19 @@
       <c r="A24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="21" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7408,19 +7400,19 @@
       <c r="A27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="21" t="s">
         <v>77</v>
       </c>
     </row>
@@ -7428,19 +7420,19 @@
       <c r="A28" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="21" t="s">
         <v>79</v>
       </c>
     </row>
@@ -7657,7 +7649,7 @@
       <c r="F40" s="6"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="19" t="s">
         <v>100</v>
       </c>
       <c r="B41" s="6"/>
@@ -7830,7 +7822,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -8020,7 +8012,7 @@
       <c r="D13" t="s">
         <v>143</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="16" t="s">
         <v>144</v>
       </c>
       <c r="F13" t="s">
@@ -8234,6 +8226,9 @@
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink display="http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnnccZenQ%3D%3D" r:id="rId1" ref="E13" tooltip="http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnnccZenQ%3D%3D"/>
+  </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
@@ -8245,7 +8240,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -8394,7 +8389,7 @@
       <c r="C13" t="s">
         <v>143</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="16" t="s">
         <v>144</v>
       </c>
       <c r="E13" t="s">
@@ -8497,6 +8492,9 @@
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink display="http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnnccZenQ%3D%3D" r:id="rId1" ref="D13" tooltip="http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnnccZenQ%3D%3D"/>
+  </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
@@ -8507,8 +8505,8 @@
   <sheetPr/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -8540,7 +8538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row ht="15.25" r="2" spans="1:6">
+    <row ht="15.25" r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -8554,7 +8552,7 @@
         <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>268</v>
       </c>
     </row>
     <row ht="29" r="3" spans="1:7">
@@ -8571,7 +8569,7 @@
         <v>133</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>134</v>
@@ -8591,7 +8589,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>53</v>
@@ -8643,10 +8641,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" t="s">
         <v>153</v>
-      </c>
-      <c r="F8" t="s">
-        <v>154</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -8657,44 +8655,45 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
         <v>155</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>156</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>157</v>
       </c>
-      <c r="E9" t="s">
-        <v>158</v>
-      </c>
       <c r="F9" t="s">
-        <v>159</v>
+        <v>267</v>
       </c>
       <c r="G9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="6" t="s">
+      <c r="D10" t="s">
         <v>161</v>
       </c>
-      <c r="D10" t="s">
-        <v>162</v>
-      </c>
-      <c r="F10" t="s">
-        <v>163</v>
+      <c r="F10"/>
+      <c r="G10" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" t="s">
         <v>164</v>
       </c>
-      <c r="D11" t="s">
-        <v>163</v>
-      </c>
       <c r="G11" t="s">
-        <v>165</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -8776,21 +8775,21 @@
         <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="E16" t="s">
         <v>143</v>
       </c>
-      <c r="F16" t="s">
-        <v>144</v>
-      </c>
-      <c r="G16" t="s">
-        <v>168</v>
+      <c r="F16" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="11" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>31</v>
@@ -8824,7 +8823,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>40</v>
@@ -8847,7 +8846,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>43</v>
@@ -9009,6 +9008,10 @@
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink display="https://gdkwebsvr:8080/i/reg?code=Qiw5KLtlFTTA3W5ZBqPoiQ%3D%3D" r:id="rId1" ref="G16"/>
+    <hyperlink display="http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnncZenQ%3D%3D" r:id="rId2" ref="F16" tooltip="http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnncZenQ%3D%3D"/>
+  </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
@@ -9019,8 +9022,8 @@
   <sheetPr/>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -9063,16 +9066,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
     </row>
     <row ht="29" r="3" spans="1:8">
@@ -9080,25 +9083,25 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -9164,16 +9167,16 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F8" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -9187,25 +9190,25 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E9" t="s">
         <v>112</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H9" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -9266,19 +9269,19 @@
         <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D13" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E13" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F13" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="G13" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>67</v>
@@ -9292,19 +9295,19 @@
         <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E14" t="s">
-        <v>191</v>
-      </c>
-      <c r="F14" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>144</v>
       </c>
       <c r="G14" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="H14" t="s">
         <v>143</v>
@@ -9312,7 +9315,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="11" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>31</v>
@@ -9350,7 +9353,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>40</v>
@@ -9376,7 +9379,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>43</v>
@@ -9402,7 +9405,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="6" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>40</v>
@@ -9428,7 +9431,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B20">
         <v>123333</v>
@@ -9591,6 +9594,9 @@
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink display="http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnnccZenQ%3D%3D" r:id="rId1" ref="F14" tooltip="http://gdkwebsvr:8080/i/reg?code=MZlysT4MmUOcKCnnccZenQ%3D%3D"/>
+  </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
@@ -9644,22 +9650,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -9719,7 +9725,7 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -9727,7 +9733,7 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -9746,22 +9752,22 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="F11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="G11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -9769,22 +9775,22 @@
         <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -9792,22 +9798,22 @@
         <v>36</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -9826,22 +9832,22 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E15" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F15" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="G15" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -9860,27 +9866,27 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D17" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E17" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F17" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G17" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="11" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>31</v>
@@ -9914,7 +9920,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>40</v>
@@ -9937,7 +9943,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>43</v>

</xml_diff>